<commit_message>
Analysis of the scans - plot
</commit_message>
<xml_diff>
--- a/notebooks/folding/geometry/TRR_demonstrator/WBScanCellAnalysis.xlsx
+++ b/notebooks/folding/geometry/TRR_demonstrator/WBScanCellAnalysis.xlsx
@@ -512,25 +512,25 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>71.58632659912109</v>
+        <v>71.58518981933594</v>
       </c>
       <c r="G2" t="n">
-        <v>1.096632331609726e-07</v>
+        <v>2.980232238769531e-08</v>
       </c>
       <c r="H2" t="n">
-        <v>-2.980232238769531e-08</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.08632659912109375</v>
+        <v>0.0851898193359375</v>
       </c>
       <c r="J2" t="n">
-        <v>1.096632331609726e-07</v>
+        <v>2.980232238769531e-08</v>
       </c>
       <c r="K2" t="n">
-        <v>-2.980232238769531e-08</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.08632659912116855</v>
+        <v>0.08518981933594272</v>
       </c>
     </row>
     <row r="3">
@@ -550,25 +550,25 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>-71.58632659912109</v>
+        <v>-71.58518981933594</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.095468178391457e-07</v>
+        <v>-2.980232238769531e-08</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.08632659912109375</v>
+        <v>-0.0851898193359375</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.095468178391457e-07</v>
+        <v>-2.980232238769531e-08</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.08632659912116326</v>
+        <v>0.08518981933594272</v>
       </c>
     </row>
     <row r="4">
@@ -588,25 +588,25 @@
         <v>118.888671875</v>
       </c>
       <c r="F4" t="n">
-        <v>318.4664001464844</v>
+        <v>319.8941040039062</v>
       </c>
       <c r="G4" t="n">
-        <v>390.2783203125</v>
+        <v>397.6437072753906</v>
       </c>
       <c r="H4" t="n">
-        <v>115.4920501708984</v>
+        <v>116.9959335327148</v>
       </c>
       <c r="I4" t="n">
-        <v>-3.033599853515625</v>
+        <v>-1.60589599609375</v>
       </c>
       <c r="J4" t="n">
-        <v>4.428955078125</v>
+        <v>11.79434204101562</v>
       </c>
       <c r="K4" t="n">
-        <v>-3.396621704101562</v>
+        <v>-1.892738342285156</v>
       </c>
       <c r="L4" t="n">
-        <v>6.352590822339579</v>
+        <v>12.05271191736926</v>
       </c>
     </row>
     <row r="5">
@@ -626,25 +626,25 @@
         <v>118.888671875</v>
       </c>
       <c r="F5" t="n">
-        <v>-327.5458374023438</v>
+        <v>-327.3821411132812</v>
       </c>
       <c r="G5" t="n">
-        <v>390.4199829101562</v>
+        <v>387.7880554199219</v>
       </c>
       <c r="H5" t="n">
-        <v>116.1202697753906</v>
+        <v>113.2660598754883</v>
       </c>
       <c r="I5" t="n">
-        <v>-6.04583740234375</v>
+        <v>-5.88214111328125</v>
       </c>
       <c r="J5" t="n">
-        <v>4.57061767578125</v>
+        <v>1.938690185546875</v>
       </c>
       <c r="K5" t="n">
-        <v>-2.768402099609375</v>
+        <v>-5.622611999511719</v>
       </c>
       <c r="L5" t="n">
-        <v>8.068875139625362</v>
+        <v>8.364918972060789</v>
       </c>
     </row>
     <row r="6">
@@ -664,25 +664,25 @@
         <v>118.888671875</v>
       </c>
       <c r="F6" t="n">
-        <v>327.8733520507812</v>
+        <v>330.939453125</v>
       </c>
       <c r="G6" t="n">
-        <v>-389.3247375488281</v>
+        <v>-386.9641723632812</v>
       </c>
       <c r="H6" t="n">
-        <v>115.4021224975586</v>
+        <v>112.4130554199219</v>
       </c>
       <c r="I6" t="n">
-        <v>6.37335205078125</v>
+        <v>9.439453125</v>
       </c>
       <c r="J6" t="n">
-        <v>-3.475372314453125</v>
+        <v>-1.11480712890625</v>
       </c>
       <c r="K6" t="n">
-        <v>-3.486549377441406</v>
+        <v>-6.475616455078125</v>
       </c>
       <c r="L6" t="n">
-        <v>8.053189160115506</v>
+        <v>11.50129030617917</v>
       </c>
     </row>
     <row r="7">
@@ -702,25 +702,25 @@
         <v>118.888671875</v>
       </c>
       <c r="F7" t="n">
-        <v>-319.3451843261719</v>
+        <v>-314.839599609375</v>
       </c>
       <c r="G7" t="n">
-        <v>-392.5595703125</v>
+        <v>-391.5144653320312</v>
       </c>
       <c r="H7" t="n">
-        <v>115.7499465942383</v>
+        <v>114.5457534790039</v>
       </c>
       <c r="I7" t="n">
-        <v>2.154815673828125</v>
+        <v>6.660400390625</v>
       </c>
       <c r="J7" t="n">
-        <v>-6.710205078125</v>
+        <v>-5.66510009765625</v>
       </c>
       <c r="K7" t="n">
-        <v>-3.138725280761719</v>
+        <v>-4.342918395996094</v>
       </c>
       <c r="L7" t="n">
-        <v>7.715029433953096</v>
+        <v>9.76295204711074</v>
       </c>
     </row>
     <row r="8">
@@ -740,25 +740,25 @@
         <v>125.0791015625</v>
       </c>
       <c r="F8" t="n">
-        <v>176.5486907958984</v>
+        <v>175.0008392333984</v>
       </c>
       <c r="G8" t="n">
-        <v>1.454917669296265</v>
+        <v>2.512862205505371</v>
       </c>
       <c r="H8" t="n">
-        <v>121.3077239990234</v>
+        <v>120.7578048706055</v>
       </c>
       <c r="I8" t="n">
-        <v>3.280120849609375</v>
+        <v>1.732269287109375</v>
       </c>
       <c r="J8" t="n">
-        <v>1.454917669296265</v>
+        <v>2.512862205505371</v>
       </c>
       <c r="K8" t="n">
-        <v>-3.771377563476562</v>
+        <v>-4.321296691894531</v>
       </c>
       <c r="L8" t="n">
-        <v>5.205695624867729</v>
+        <v>5.290447849312793</v>
       </c>
     </row>
     <row r="9">
@@ -778,25 +778,25 @@
         <v>125.0791015625</v>
       </c>
       <c r="F9" t="n">
-        <v>-176.6955871582031</v>
+        <v>-180.8824920654297</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.735987901687622</v>
+        <v>-1.754476547241211</v>
       </c>
       <c r="H9" t="n">
-        <v>122.4498748779297</v>
+        <v>120.9316253662109</v>
       </c>
       <c r="I9" t="n">
-        <v>-3.427017211914062</v>
+        <v>-7.613922119140625</v>
       </c>
       <c r="J9" t="n">
-        <v>-1.735987901687622</v>
+        <v>-1.754476547241211</v>
       </c>
       <c r="K9" t="n">
-        <v>-2.629226684570312</v>
+        <v>-4.147476196289062</v>
       </c>
       <c r="L9" t="n">
-        <v>4.65520503570118</v>
+        <v>8.845991001009592</v>
       </c>
     </row>
     <row r="10">
@@ -816,25 +816,25 @@
         <v>-6.1259765625</v>
       </c>
       <c r="F10" t="n">
-        <v>-429.871315464814</v>
+        <v>-437.4225924276399</v>
       </c>
       <c r="G10" t="n">
-        <v>383.3326421708483</v>
+        <v>381.9615940344092</v>
       </c>
       <c r="H10" t="n">
-        <v>-7.909347425303196</v>
+        <v>-6.630470556753934</v>
       </c>
       <c r="I10" t="n">
-        <v>-6.602746370961995</v>
+        <v>-14.1540233337879</v>
       </c>
       <c r="J10" t="n">
-        <v>1.49603328412951</v>
+        <v>0.1249851476904382</v>
       </c>
       <c r="K10" t="n">
-        <v>-1.783370862803196</v>
+        <v>-0.5044939942539344</v>
       </c>
       <c r="L10" t="n">
-        <v>7.001056124669373</v>
+        <v>14.16356282899165</v>
       </c>
     </row>
     <row r="11">
@@ -854,25 +854,25 @@
         <v>-6.1259765625</v>
       </c>
       <c r="F11" t="n">
-        <v>-503.2149682387073</v>
+        <v>-506.7551674841308</v>
       </c>
       <c r="G11" t="n">
-        <v>383.3326421708483</v>
+        <v>381.9615940344092</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.909347425303196</v>
+        <v>-6.630470556753934</v>
       </c>
       <c r="I11" t="n">
-        <v>-8.446399144855377</v>
+        <v>-11.98659839027886</v>
       </c>
       <c r="J11" t="n">
-        <v>1.49603328412951</v>
+        <v>0.1249851476904382</v>
       </c>
       <c r="K11" t="n">
-        <v>-1.783370862803196</v>
+        <v>-0.5044939942539344</v>
       </c>
       <c r="L11" t="n">
-        <v>8.761289045325031</v>
+        <v>11.99786132805415</v>
       </c>
     </row>
     <row r="12">
@@ -892,25 +892,25 @@
         <v>125.0791015625</v>
       </c>
       <c r="F12" t="n">
-        <v>-503.2149682387073</v>
+        <v>-506.7551674841308</v>
       </c>
       <c r="G12" t="n">
-        <v>-2.083700517087247</v>
+        <v>-3.757515036852001</v>
       </c>
       <c r="H12" t="n">
-        <v>120.4774682284593</v>
+        <v>122.4495703003242</v>
       </c>
       <c r="I12" t="n">
-        <v>-8.446413977425891</v>
+        <v>-11.98661322284937</v>
       </c>
       <c r="J12" t="n">
-        <v>-2.083692887692715</v>
+        <v>-3.75750740745747</v>
       </c>
       <c r="K12" t="n">
-        <v>-4.601633334040699</v>
+        <v>-2.629531262175803</v>
       </c>
       <c r="L12" t="n">
-        <v>9.841682501952153</v>
+        <v>12.83402482193505</v>
       </c>
     </row>
     <row r="13">
@@ -930,25 +930,25 @@
         <v>-6.1259765625</v>
       </c>
       <c r="F13" t="n">
-        <v>-425.284358442269</v>
+        <v>-428.5609914843379</v>
       </c>
       <c r="G13" t="n">
-        <v>-390.4386353430185</v>
+        <v>-392.6309405816843</v>
       </c>
       <c r="H13" t="n">
-        <v>-5.937140856427703</v>
+        <v>-2.331833789497878</v>
       </c>
       <c r="I13" t="n">
-        <v>-2.015789348416945</v>
+        <v>-5.29242239048591</v>
       </c>
       <c r="J13" t="n">
-        <v>-8.602026456299711</v>
+        <v>-10.79433169496554</v>
       </c>
       <c r="K13" t="n">
-        <v>0.1888357060722967</v>
+        <v>3.794142773002122</v>
       </c>
       <c r="L13" t="n">
-        <v>8.837076709860519</v>
+        <v>12.60646068022973</v>
       </c>
     </row>
     <row r="14">
@@ -968,25 +968,25 @@
         <v>-6.1259765625</v>
       </c>
       <c r="F14" t="n">
-        <v>-503.2149682387073</v>
+        <v>-506.7551674841308</v>
       </c>
       <c r="G14" t="n">
-        <v>-390.4386353430185</v>
+        <v>-392.6309405816843</v>
       </c>
       <c r="H14" t="n">
-        <v>-5.937140856427703</v>
+        <v>-2.331833789497878</v>
       </c>
       <c r="I14" t="n">
-        <v>-8.446399144855377</v>
+        <v>-11.98659839027886</v>
       </c>
       <c r="J14" t="n">
-        <v>-8.602026456299711</v>
+        <v>-10.79433169496554</v>
       </c>
       <c r="K14" t="n">
-        <v>0.1888357060722967</v>
+        <v>3.794142773002122</v>
       </c>
       <c r="L14" t="n">
-        <v>12.057038466928</v>
+        <v>16.57080737600608</v>
       </c>
     </row>
     <row r="15">
@@ -1006,25 +1006,25 @@
         <v>-6.1259765625</v>
       </c>
       <c r="F15" t="n">
-        <v>502.6869373237507</v>
+        <v>501.180500954079</v>
       </c>
       <c r="G15" t="n">
-        <v>391.1160998887622</v>
+        <v>394.735955483039</v>
       </c>
       <c r="H15" t="n">
-        <v>-10.50795155823329</v>
+        <v>-12.07237651241684</v>
       </c>
       <c r="I15" t="n">
-        <v>7.918368229898761</v>
+        <v>6.411931860227071</v>
       </c>
       <c r="J15" t="n">
-        <v>9.279491002043414</v>
+        <v>12.8993465963203</v>
       </c>
       <c r="K15" t="n">
-        <v>-4.381974995733287</v>
+        <v>-5.946399949916838</v>
       </c>
       <c r="L15" t="n">
-        <v>12.96191396146829</v>
+        <v>15.58414852202603</v>
       </c>
     </row>
     <row r="16">
@@ -1044,25 +1044,25 @@
         <v>-6.1259765625</v>
       </c>
       <c r="F16" t="n">
-        <v>421.8202901663933</v>
+        <v>415.5005639093517</v>
       </c>
       <c r="G16" t="n">
-        <v>391.1160998887622</v>
+        <v>394.735955483039</v>
       </c>
       <c r="H16" t="n">
-        <v>-10.50795155823329</v>
+        <v>-12.07237651241684</v>
       </c>
       <c r="I16" t="n">
-        <v>-1.448278927458716</v>
+        <v>-7.768005184500282</v>
       </c>
       <c r="J16" t="n">
-        <v>9.279491002043414</v>
+        <v>12.8993465963203</v>
       </c>
       <c r="K16" t="n">
-        <v>-4.381974995733287</v>
+        <v>-5.946399949916838</v>
       </c>
       <c r="L16" t="n">
-        <v>10.36379129334229</v>
+        <v>16.18933968767085</v>
       </c>
     </row>
     <row r="17">
@@ -1082,25 +1082,25 @@
         <v>125.0791015625</v>
       </c>
       <c r="F17" t="n">
-        <v>502.6869373237507</v>
+        <v>501.180500954079</v>
       </c>
       <c r="G17" t="n">
-        <v>9.255529457693264</v>
+        <v>11.92230898046362</v>
       </c>
       <c r="H17" t="n">
-        <v>119.0693494823783</v>
+        <v>115.3838192856772</v>
       </c>
       <c r="I17" t="n">
-        <v>7.918383062469275</v>
+        <v>6.411946692797585</v>
       </c>
       <c r="J17" t="n">
-        <v>9.255537087087795</v>
+        <v>11.92231660985816</v>
       </c>
       <c r="K17" t="n">
-        <v>-6.009752080121729</v>
+        <v>-9.695282276822837</v>
       </c>
       <c r="L17" t="n">
-        <v>13.58244739209342</v>
+        <v>16.65092166110491</v>
       </c>
     </row>
     <row r="18">
@@ -1120,25 +1120,25 @@
         <v>-6.1259765625</v>
       </c>
       <c r="F18" t="n">
-        <v>502.6869373237507</v>
+        <v>501.180500954079</v>
       </c>
       <c r="G18" t="n">
-        <v>-381.0897010535917</v>
+        <v>-377.2416097670476</v>
       </c>
       <c r="H18" t="n">
-        <v>-3.234973593499063</v>
+        <v>-10.06250876749758</v>
       </c>
       <c r="I18" t="n">
-        <v>7.918368229898761</v>
+        <v>6.411931860227071</v>
       </c>
       <c r="J18" t="n">
-        <v>0.746907833127068</v>
+        <v>4.594999119671172</v>
       </c>
       <c r="K18" t="n">
-        <v>2.891002969000937</v>
+        <v>-3.936532204997576</v>
       </c>
       <c r="L18" t="n">
-        <v>8.4626429029133</v>
+        <v>8.816074687237904</v>
       </c>
     </row>
     <row r="19">
@@ -1158,25 +1158,25 @@
         <v>-6.1259765625</v>
       </c>
       <c r="F19" t="n">
-        <v>436.3910956073344</v>
+        <v>435.7603124203657</v>
       </c>
       <c r="G19" t="n">
-        <v>-381.0897010535917</v>
+        <v>-377.2416097670476</v>
       </c>
       <c r="H19" t="n">
-        <v>-3.234973593499063</v>
+        <v>-10.06250876749758</v>
       </c>
       <c r="I19" t="n">
-        <v>13.1225265134824</v>
+        <v>12.4917433265137</v>
       </c>
       <c r="J19" t="n">
-        <v>0.746907833127068</v>
+        <v>4.594999119671172</v>
       </c>
       <c r="K19" t="n">
-        <v>2.891002969000937</v>
+        <v>-3.936532204997576</v>
       </c>
       <c r="L19" t="n">
-        <v>13.45795198293586</v>
+        <v>13.87998393537476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update with scan code and analytical geometry
</commit_message>
<xml_diff>
--- a/notebooks/folding/geometry/TRR_demonstrator/WBScanCellAnalysis.xlsx
+++ b/notebooks/folding/geometry/TRR_demonstrator/WBScanCellAnalysis.xlsx
@@ -500,7 +500,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
         <v>71.5</v>
@@ -509,28 +509,28 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>-0.0003960461763199419</v>
       </c>
       <c r="F2" t="n">
-        <v>71.58518981933594</v>
+        <v>8948.2294921875</v>
       </c>
       <c r="G2" t="n">
-        <v>2.980232238769531e-08</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>-63.4466552734375</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0851898193359375</v>
+        <v>8876.7294921875</v>
       </c>
       <c r="J2" t="n">
-        <v>2.980232238769531e-08</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>-63.44625922726118</v>
       </c>
       <c r="L2" t="n">
-        <v>0.08518981933594272</v>
+        <v>8877.248162495487</v>
       </c>
     </row>
     <row r="3">
@@ -547,28 +547,28 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>-0.0003960461763199419</v>
       </c>
       <c r="F3" t="n">
-        <v>-71.58518981933594</v>
+        <v>-9078.669921875</v>
       </c>
       <c r="G3" t="n">
-        <v>-2.980232238769531e-08</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>-0.000244140625</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.0851898193359375</v>
+        <v>-9007.169921875</v>
       </c>
       <c r="J3" t="n">
-        <v>-2.980232238769531e-08</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>0.0001519055513199419</v>
       </c>
       <c r="L3" t="n">
-        <v>0.08518981933594272</v>
+        <v>9007.169921875002</v>
       </c>
     </row>
     <row r="4">
@@ -576,7 +576,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
         <v>321.5</v>
@@ -585,28 +585,28 @@
         <v>385.849365234375</v>
       </c>
       <c r="E4" t="n">
-        <v>118.888671875</v>
+        <v>118.8882751464844</v>
       </c>
       <c r="F4" t="n">
-        <v>319.8941040039062</v>
+        <v>8948.2294921875</v>
       </c>
       <c r="G4" t="n">
-        <v>397.6437072753906</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="H4" t="n">
-        <v>116.9959335327148</v>
+        <v>-63.4466552734375</v>
       </c>
       <c r="I4" t="n">
-        <v>-1.60589599609375</v>
+        <v>8626.7294921875</v>
       </c>
       <c r="J4" t="n">
-        <v>11.79434204101562</v>
+        <v>-313.8560791015625</v>
       </c>
       <c r="K4" t="n">
-        <v>-1.892738342285156</v>
+        <v>-182.3349304199219</v>
       </c>
       <c r="L4" t="n">
-        <v>12.05271191736926</v>
+        <v>8634.362361901303</v>
       </c>
     </row>
     <row r="5">
@@ -614,7 +614,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
         <v>-321.5</v>
@@ -623,28 +623,28 @@
         <v>385.849365234375</v>
       </c>
       <c r="E5" t="n">
-        <v>118.888671875</v>
+        <v>118.8882751464844</v>
       </c>
       <c r="F5" t="n">
-        <v>-327.3821411132812</v>
+        <v>-9078.669921875</v>
       </c>
       <c r="G5" t="n">
-        <v>387.7880554199219</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>113.2660598754883</v>
+        <v>-0.000244140625</v>
       </c>
       <c r="I5" t="n">
-        <v>-5.88214111328125</v>
+        <v>-8757.169921875</v>
       </c>
       <c r="J5" t="n">
-        <v>1.938690185546875</v>
+        <v>-385.849365234375</v>
       </c>
       <c r="K5" t="n">
-        <v>-5.622611999511719</v>
+        <v>-118.8885192871094</v>
       </c>
       <c r="L5" t="n">
-        <v>8.364918972060789</v>
+        <v>8766.472452090537</v>
       </c>
     </row>
     <row r="6">
@@ -652,7 +652,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>321.5</v>
@@ -661,28 +661,28 @@
         <v>-385.849365234375</v>
       </c>
       <c r="E6" t="n">
-        <v>118.888671875</v>
+        <v>118.8882751464844</v>
       </c>
       <c r="F6" t="n">
-        <v>330.939453125</v>
+        <v>8948.2294921875</v>
       </c>
       <c r="G6" t="n">
-        <v>-386.9641723632812</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="H6" t="n">
-        <v>112.4130554199219</v>
+        <v>-63.4466552734375</v>
       </c>
       <c r="I6" t="n">
-        <v>9.439453125</v>
+        <v>8626.7294921875</v>
       </c>
       <c r="J6" t="n">
-        <v>-1.11480712890625</v>
+        <v>457.8426513671875</v>
       </c>
       <c r="K6" t="n">
-        <v>-6.475616455078125</v>
+        <v>-182.3349304199219</v>
       </c>
       <c r="L6" t="n">
-        <v>11.50129030617917</v>
+        <v>8640.794387765502</v>
       </c>
     </row>
     <row r="7">
@@ -690,7 +690,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
         <v>-321.5</v>
@@ -699,28 +699,28 @@
         <v>-385.849365234375</v>
       </c>
       <c r="E7" t="n">
-        <v>118.888671875</v>
+        <v>118.8882751464844</v>
       </c>
       <c r="F7" t="n">
-        <v>-314.839599609375</v>
+        <v>-9078.669921875</v>
       </c>
       <c r="G7" t="n">
-        <v>-391.5144653320312</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>114.5457534790039</v>
+        <v>-0.000244140625</v>
       </c>
       <c r="I7" t="n">
-        <v>6.660400390625</v>
+        <v>-8757.169921875</v>
       </c>
       <c r="J7" t="n">
-        <v>-5.66510009765625</v>
+        <v>385.849365234375</v>
       </c>
       <c r="K7" t="n">
-        <v>-4.342918395996094</v>
+        <v>-118.8885192871094</v>
       </c>
       <c r="L7" t="n">
-        <v>9.76295204711074</v>
+        <v>8766.472452090537</v>
       </c>
     </row>
     <row r="8">
@@ -737,28 +737,28 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>125.0791015625</v>
+        <v>125.0787048339844</v>
       </c>
       <c r="F8" t="n">
-        <v>175.0008392333984</v>
+        <v>8948.2294921875</v>
       </c>
       <c r="G8" t="n">
-        <v>2.512862205505371</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="H8" t="n">
-        <v>120.7578048706055</v>
+        <v>-63.4466552734375</v>
       </c>
       <c r="I8" t="n">
-        <v>1.732269287109375</v>
+        <v>8774.960922241211</v>
       </c>
       <c r="J8" t="n">
-        <v>2.512862205505371</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="K8" t="n">
-        <v>-4.321296691894531</v>
+        <v>-188.5253601074219</v>
       </c>
       <c r="L8" t="n">
-        <v>5.290447849312793</v>
+        <v>8777.281129798233</v>
       </c>
     </row>
     <row r="9">
@@ -766,7 +766,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" t="n">
         <v>-173.2685699462891</v>
@@ -775,28 +775,28 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>125.0791015625</v>
+        <v>125.0787048339844</v>
       </c>
       <c r="F9" t="n">
-        <v>-180.8824920654297</v>
+        <v>-9078.669921875</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.754476547241211</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>120.9316253662109</v>
+        <v>-0.000244140625</v>
       </c>
       <c r="I9" t="n">
-        <v>-7.613922119140625</v>
+        <v>-8905.401351928711</v>
       </c>
       <c r="J9" t="n">
-        <v>-1.754476547241211</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>-4.147476196289062</v>
+        <v>-125.0789489746094</v>
       </c>
       <c r="L9" t="n">
-        <v>8.845991001009592</v>
+        <v>8906.279693699851</v>
       </c>
     </row>
     <row r="10">
@@ -804,7 +804,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C10" t="n">
         <v>-423.268569093852</v>
@@ -813,28 +813,28 @@
         <v>381.8366088867188</v>
       </c>
       <c r="E10" t="n">
-        <v>-6.1259765625</v>
+        <v>-6.126372814178467</v>
       </c>
       <c r="F10" t="n">
-        <v>-437.4225924276399</v>
+        <v>-9078.669921875</v>
       </c>
       <c r="G10" t="n">
-        <v>381.9615940344092</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>-6.630470556753934</v>
+        <v>-0.000244140625</v>
       </c>
       <c r="I10" t="n">
-        <v>-14.1540233337879</v>
+        <v>-8655.401352781148</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1249851476904382</v>
+        <v>-381.8366088867188</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.5044939942539344</v>
+        <v>6.126128673553467</v>
       </c>
       <c r="L10" t="n">
-        <v>14.16356282899165</v>
+        <v>8663.821864689067</v>
       </c>
     </row>
     <row r="11">
@@ -842,7 +842,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
         <v>-494.768569093852</v>
@@ -851,28 +851,28 @@
         <v>381.8366088867188</v>
       </c>
       <c r="E11" t="n">
-        <v>-6.1259765625</v>
+        <v>-6.126372814178467</v>
       </c>
       <c r="F11" t="n">
-        <v>-506.7551674841308</v>
+        <v>-9078.669921875</v>
       </c>
       <c r="G11" t="n">
-        <v>381.9615940344092</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>-6.630470556753934</v>
+        <v>-0.000244140625</v>
       </c>
       <c r="I11" t="n">
-        <v>-11.98659839027886</v>
+        <v>-8583.901352781148</v>
       </c>
       <c r="J11" t="n">
-        <v>0.1249851476904382</v>
+        <v>-381.8366088867188</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.5044939942539344</v>
+        <v>6.126128673553467</v>
       </c>
       <c r="L11" t="n">
-        <v>11.99786132805415</v>
+        <v>8592.391934706926</v>
       </c>
     </row>
     <row r="12">
@@ -880,7 +880,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
         <v>-494.7685542612815</v>
@@ -889,28 +889,28 @@
         <v>-7.62939453125e-06</v>
       </c>
       <c r="E12" t="n">
-        <v>125.0791015625</v>
+        <v>125.0787048339844</v>
       </c>
       <c r="F12" t="n">
-        <v>-506.7551674841308</v>
+        <v>-9078.669921875</v>
       </c>
       <c r="G12" t="n">
-        <v>-3.757515036852001</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>122.4495703003242</v>
+        <v>-0.000244140625</v>
       </c>
       <c r="I12" t="n">
-        <v>-11.98661322284937</v>
+        <v>-8583.901367613718</v>
       </c>
       <c r="J12" t="n">
-        <v>-3.75750740745747</v>
+        <v>7.62939453125e-06</v>
       </c>
       <c r="K12" t="n">
-        <v>-2.629531262175803</v>
+        <v>-125.0789489746094</v>
       </c>
       <c r="L12" t="n">
-        <v>12.83402482193505</v>
+        <v>8584.812603219552</v>
       </c>
     </row>
     <row r="13">
@@ -918,7 +918,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
         <v>-423.268569093852</v>
@@ -927,28 +927,28 @@
         <v>-381.8366088867188</v>
       </c>
       <c r="E13" t="n">
-        <v>-6.1259765625</v>
+        <v>-6.126372814178467</v>
       </c>
       <c r="F13" t="n">
-        <v>-428.5609914843379</v>
+        <v>-9078.669921875</v>
       </c>
       <c r="G13" t="n">
-        <v>-392.6309405816843</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>-2.331833789497878</v>
+        <v>-0.000244140625</v>
       </c>
       <c r="I13" t="n">
-        <v>-5.29242239048591</v>
+        <v>-8655.401352781148</v>
       </c>
       <c r="J13" t="n">
-        <v>-10.79433169496554</v>
+        <v>381.8366088867188</v>
       </c>
       <c r="K13" t="n">
-        <v>3.794142773002122</v>
+        <v>6.126128673553467</v>
       </c>
       <c r="L13" t="n">
-        <v>12.60646068022973</v>
+        <v>8663.821864689067</v>
       </c>
     </row>
     <row r="14">
@@ -956,7 +956,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
         <v>-494.768569093852</v>
@@ -965,28 +965,28 @@
         <v>-381.8366088867188</v>
       </c>
       <c r="E14" t="n">
-        <v>-6.1259765625</v>
+        <v>-6.126372814178467</v>
       </c>
       <c r="F14" t="n">
-        <v>-506.7551674841308</v>
+        <v>-9078.669921875</v>
       </c>
       <c r="G14" t="n">
-        <v>-392.6309405816843</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>-2.331833789497878</v>
+        <v>-0.000244140625</v>
       </c>
       <c r="I14" t="n">
-        <v>-11.98659839027886</v>
+        <v>-8583.901352781148</v>
       </c>
       <c r="J14" t="n">
-        <v>-10.79433169496554</v>
+        <v>381.8366088867188</v>
       </c>
       <c r="K14" t="n">
-        <v>3.794142773002122</v>
+        <v>6.126128673553467</v>
       </c>
       <c r="L14" t="n">
-        <v>16.57080737600608</v>
+        <v>8592.391934706926</v>
       </c>
     </row>
     <row r="15">
@@ -994,7 +994,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
         <v>494.768569093852</v>
@@ -1003,28 +1003,28 @@
         <v>381.8366088867188</v>
       </c>
       <c r="E15" t="n">
-        <v>-6.1259765625</v>
+        <v>-6.126372814178467</v>
       </c>
       <c r="F15" t="n">
-        <v>501.180500954079</v>
+        <v>8948.2294921875</v>
       </c>
       <c r="G15" t="n">
-        <v>394.735955483039</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="H15" t="n">
-        <v>-12.07237651241684</v>
+        <v>-63.4466552734375</v>
       </c>
       <c r="I15" t="n">
-        <v>6.411931860227071</v>
+        <v>8453.460923093648</v>
       </c>
       <c r="J15" t="n">
-        <v>12.8993465963203</v>
+        <v>-309.8433227539062</v>
       </c>
       <c r="K15" t="n">
-        <v>-5.946399949916838</v>
+        <v>-57.32028245925903</v>
       </c>
       <c r="L15" t="n">
-        <v>15.58414852202603</v>
+        <v>8459.33153846731</v>
       </c>
     </row>
     <row r="16">
@@ -1032,7 +1032,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
         <v>423.268569093852</v>
@@ -1041,28 +1041,28 @@
         <v>381.8366088867188</v>
       </c>
       <c r="E16" t="n">
-        <v>-6.1259765625</v>
+        <v>-6.126372814178467</v>
       </c>
       <c r="F16" t="n">
-        <v>415.5005639093517</v>
+        <v>8948.2294921875</v>
       </c>
       <c r="G16" t="n">
-        <v>394.735955483039</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="H16" t="n">
-        <v>-12.07237651241684</v>
+        <v>-63.4466552734375</v>
       </c>
       <c r="I16" t="n">
-        <v>-7.768005184500282</v>
+        <v>8524.960923093648</v>
       </c>
       <c r="J16" t="n">
-        <v>12.8993465963203</v>
+        <v>-309.8433227539062</v>
       </c>
       <c r="K16" t="n">
-        <v>-5.946399949916838</v>
+        <v>-57.32028245925903</v>
       </c>
       <c r="L16" t="n">
-        <v>16.18933968767085</v>
+        <v>8530.782334564052</v>
       </c>
     </row>
     <row r="17">
@@ -1070,7 +1070,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
         <v>494.7685542612815</v>
@@ -1079,28 +1079,28 @@
         <v>-7.62939453125e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>125.0791015625</v>
+        <v>125.0787048339844</v>
       </c>
       <c r="F17" t="n">
-        <v>501.180500954079</v>
+        <v>8948.2294921875</v>
       </c>
       <c r="G17" t="n">
-        <v>11.92230898046362</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="H17" t="n">
-        <v>115.3838192856772</v>
+        <v>-63.4466552734375</v>
       </c>
       <c r="I17" t="n">
-        <v>6.411946692797585</v>
+        <v>8453.460937926218</v>
       </c>
       <c r="J17" t="n">
-        <v>11.92231660985816</v>
+        <v>71.99329376220703</v>
       </c>
       <c r="K17" t="n">
-        <v>-9.695282276822837</v>
+        <v>-188.5253601074219</v>
       </c>
       <c r="L17" t="n">
-        <v>16.65092166110491</v>
+        <v>8455.869362448475</v>
       </c>
     </row>
     <row r="18">
@@ -1108,7 +1108,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C18" t="n">
         <v>494.768569093852</v>
@@ -1117,28 +1117,28 @@
         <v>-381.8366088867188</v>
       </c>
       <c r="E18" t="n">
-        <v>-6.1259765625</v>
+        <v>-6.126372814178467</v>
       </c>
       <c r="F18" t="n">
-        <v>501.180500954079</v>
+        <v>8948.2294921875</v>
       </c>
       <c r="G18" t="n">
-        <v>-377.2416097670476</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="H18" t="n">
-        <v>-10.06250876749758</v>
+        <v>-63.4466552734375</v>
       </c>
       <c r="I18" t="n">
-        <v>6.411931860227071</v>
+        <v>8453.460923093648</v>
       </c>
       <c r="J18" t="n">
-        <v>4.594999119671172</v>
+        <v>453.8298950195312</v>
       </c>
       <c r="K18" t="n">
-        <v>-3.936532204997576</v>
+        <v>-57.32028245925903</v>
       </c>
       <c r="L18" t="n">
-        <v>8.816074687237904</v>
+        <v>8465.828297731177</v>
       </c>
     </row>
     <row r="19">
@@ -1146,7 +1146,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C19" t="n">
         <v>423.268569093852</v>
@@ -1155,28 +1155,28 @@
         <v>-381.8366088867188</v>
       </c>
       <c r="E19" t="n">
-        <v>-6.1259765625</v>
+        <v>-6.126372814178467</v>
       </c>
       <c r="F19" t="n">
-        <v>435.7603124203657</v>
+        <v>8948.2294921875</v>
       </c>
       <c r="G19" t="n">
-        <v>-377.2416097670476</v>
+        <v>71.9932861328125</v>
       </c>
       <c r="H19" t="n">
-        <v>-10.06250876749758</v>
+        <v>-63.4466552734375</v>
       </c>
       <c r="I19" t="n">
-        <v>12.4917433265137</v>
+        <v>8524.960923093648</v>
       </c>
       <c r="J19" t="n">
-        <v>4.594999119671172</v>
+        <v>453.8298950195312</v>
       </c>
       <c r="K19" t="n">
-        <v>-3.936532204997576</v>
+        <v>-57.32028245925903</v>
       </c>
       <c r="L19" t="n">
-        <v>13.87998393537476</v>
+        <v>8537.224720520619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>